<commit_message>
Partial Project, Code and Folder cleanup
</commit_message>
<xml_diff>
--- a/src/PerceptronDS1ValidationResults.xlsx
+++ b/src/PerceptronDS1ValidationResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\eclipse\NikhilWorkspace\LearningAlgorithms\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E70627A1-BFCB-46E2-8803-C0B976D49100}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E181A384-E7A8-4ADA-92B0-6C453C081FC6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21268" windowHeight="8097" xr2:uid="{C8BCA09A-6FAF-46B9-B34E-BE9E36FC53C0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Perceptron:</t>
   </si>
@@ -40,6 +40,27 @@
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>DS2</t>
+  </si>
+  <si>
+    <t>DS3</t>
+  </si>
+  <si>
+    <t>For Validation Set</t>
+  </si>
+  <si>
+    <t>For Test Set</t>
+  </si>
+  <si>
+    <t>DS1</t>
+  </si>
+  <si>
+    <t>Accuracy of Ham</t>
+  </si>
+  <si>
+    <t>Accuracy of Spam</t>
   </si>
 </sst>
 </file>
@@ -419,13 +440,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A344AB49-53FD-4E0F-B03D-FFFB13EAE874}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -506,6 +531,218 @@
         <v>0.85</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.82220000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>0.81481400000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>0.83699999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>250</v>
+      </c>
+      <c r="C21">
+        <v>0.84440000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>500</v>
+      </c>
+      <c r="C22">
+        <v>0.86666699999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>750</v>
+      </c>
+      <c r="C23">
+        <v>0.84443999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1000</v>
+      </c>
+      <c r="C24">
+        <v>0.82962000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.78259999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>50</v>
+      </c>
+      <c r="C31">
+        <v>0.91920000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>100</v>
+      </c>
+      <c r="C32">
+        <v>0.89439999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>250</v>
+      </c>
+      <c r="C33">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>500</v>
+      </c>
+      <c r="C34">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>750</v>
+      </c>
+      <c r="C35">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1000</v>
+      </c>
+      <c r="C36">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>750</v>
+      </c>
+      <c r="C44">
+        <v>0.91954022988505701</v>
+      </c>
+      <c r="E44">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>750</v>
+      </c>
+      <c r="C47">
+        <v>0.91205211726384305</v>
+      </c>
+      <c r="E47">
+        <v>0.88590604026845599</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>750</v>
+      </c>
+      <c r="C50">
+        <v>0.88157894736842102</v>
+      </c>
+      <c r="E50">
+        <v>0.93861892583120199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>